<commit_message>
Enhanced program_counter increment process
</commit_message>
<xml_diff>
--- a/UM/HW7/labnotes.xlsx
+++ b/UM/HW7/labnotes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7040" yWindow="980" windowWidth="20240" windowHeight="12680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7000" yWindow="1900" windowWidth="20240" windowHeight="12680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>Benchmark</t>
   </si>
@@ -68,10 +68,22 @@
     <t>Compiles with optimiazation flag -O2 turned on and linked against -lcii-O2</t>
   </si>
   <si>
-    <t>Eliminate function call to bitpack_getu. Removes assertions, and creates static mask.</t>
-  </si>
-  <si>
     <t>Seq_get , Uarray_at</t>
+  </si>
+  <si>
+    <t>Callgrind</t>
+  </si>
+  <si>
+    <t>callgrind.out.27941</t>
+  </si>
+  <si>
+    <t>segmented_load, segmented_store</t>
+  </si>
+  <si>
+    <t>Eliminate function call to bitpack_getu. Created smaller verstion of bitpack_getus using local variables for masks and shift values. Removes assertions, and creates static mask.</t>
+  </si>
+  <si>
+    <t>Changed program_counter to directly point to next index by incrementing by +1, rather than extracting array from sequence</t>
   </si>
 </sst>
 </file>
@@ -81,7 +93,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -104,13 +116,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -131,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -140,6 +164,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -396,6 +435,43 @@
       </right>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -404,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -424,176 +500,198 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -913,7 +1011,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -925,7 +1023,8 @@
     <col min="5" max="5" width="14.6640625" style="5" customWidth="1"/>
     <col min="6" max="6" width="37.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="1025" width="21" style="2"/>
+    <col min="8" max="8" width="27" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="1025" width="21" style="2"/>
     <col min="1026" max="16384" width="21" style="3"/>
   </cols>
   <sheetData>
@@ -951,6 +1050,9 @@
       <c r="G1" s="63" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="64" t="s">
+        <v>15</v>
+      </c>
       <c r="AMJ1" s="2"/>
     </row>
     <row r="2" spans="1:1024" x14ac:dyDescent="0.15">
@@ -975,6 +1077,7 @@
       <c r="G2" s="42" t="s">
         <v>9</v>
       </c>
+      <c r="H2" s="65"/>
     </row>
     <row r="3" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A3" s="19" t="s">
@@ -992,6 +1095,7 @@
       </c>
       <c r="F3" s="41"/>
       <c r="G3" s="43"/>
+      <c r="H3" s="66"/>
     </row>
     <row r="4" spans="1:1024" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
@@ -1011,6 +1115,7 @@
       </c>
       <c r="F4" s="57"/>
       <c r="G4" s="44"/>
+      <c r="H4" s="66"/>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A5" s="37" t="s">
@@ -1034,6 +1139,7 @@
       <c r="G5" s="55" t="s">
         <v>9</v>
       </c>
+      <c r="H5" s="66"/>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
@@ -1053,6 +1159,7 @@
       </c>
       <c r="F6" s="50"/>
       <c r="G6" s="51"/>
+      <c r="H6" s="66"/>
     </row>
     <row r="7" spans="1:1024" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
@@ -1074,6 +1181,7 @@
       </c>
       <c r="F7" s="52"/>
       <c r="G7" s="53"/>
+      <c r="H7" s="66"/>
     </row>
     <row r="8" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A8" s="45" t="s">
@@ -1097,6 +1205,7 @@
       <c r="G8" s="49" t="s">
         <v>9</v>
       </c>
+      <c r="H8" s="66"/>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A9" s="19" t="s">
@@ -1116,6 +1225,7 @@
       </c>
       <c r="F9" s="41"/>
       <c r="G9" s="43"/>
+      <c r="H9" s="66"/>
     </row>
     <row r="10" spans="1:1024" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
@@ -1137,8 +1247,9 @@
       </c>
       <c r="F10" s="57"/>
       <c r="G10" s="44"/>
-    </row>
-    <row r="11" spans="1:1024" x14ac:dyDescent="0.15">
+      <c r="H10" s="66"/>
+    </row>
+    <row r="11" spans="1:1024" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="37" t="s">
         <v>7</v>
       </c>
@@ -1155,13 +1266,14 @@
         <v>0.56497840596780535</v>
       </c>
       <c r="F11" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="55" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1024" x14ac:dyDescent="0.15">
+      <c r="H11" s="66"/>
+    </row>
+    <row r="12" spans="1:1024" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -1179,8 +1291,9 @@
       </c>
       <c r="F12" s="50"/>
       <c r="G12" s="51"/>
-    </row>
-    <row r="13" spans="1:1024" ht="17" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="66"/>
+    </row>
+    <row r="13" spans="1:1024" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
@@ -1200,8 +1313,9 @@
       </c>
       <c r="F13" s="52"/>
       <c r="G13" s="53"/>
-    </row>
-    <row r="14" spans="1:1024" x14ac:dyDescent="0.15">
+      <c r="H13" s="66"/>
+    </row>
+    <row r="14" spans="1:1024" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="45" t="s">
         <v>7</v>
       </c>
@@ -1215,12 +1329,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F14" s="29"/>
+      <c r="F14" s="69" t="s">
+        <v>19</v>
+      </c>
       <c r="G14" s="49" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1024" x14ac:dyDescent="0.15">
+        <v>17</v>
+      </c>
+      <c r="H14" s="66"/>
+    </row>
+    <row r="15" spans="1:1024" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="19" t="s">
         <v>10</v>
       </c>
@@ -1234,10 +1351,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F15" s="30"/>
+      <c r="F15" s="70"/>
       <c r="G15" s="43"/>
-    </row>
-    <row r="16" spans="1:1024" ht="17" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="H15" s="66"/>
+    </row>
+    <row r="16" spans="1:1024" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>11</v>
       </c>
@@ -1251,10 +1369,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F16" s="31"/>
+      <c r="F16" s="71"/>
       <c r="G16" s="44"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H16" s="68" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="37" t="s">
         <v>7</v>
       </c>
@@ -1270,8 +1391,9 @@
       </c>
       <c r="F17" s="27"/>
       <c r="G17" s="32"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H17" s="66"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>10</v>
       </c>
@@ -1287,8 +1409,9 @@
       </c>
       <c r="F18" s="27"/>
       <c r="G18" s="32"/>
-    </row>
-    <row r="19" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="H18" s="66"/>
+    </row>
+    <row r="19" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>11</v>
       </c>
@@ -1304,8 +1427,9 @@
       </c>
       <c r="F19" s="28"/>
       <c r="G19" s="33"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H19" s="66"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="15" t="s">
         <v>7</v>
       </c>
@@ -1321,8 +1445,9 @@
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="34"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H20" s="66"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="19" t="s">
         <v>10</v>
       </c>
@@ -1338,8 +1463,9 @@
       </c>
       <c r="F21" s="30"/>
       <c r="G21" s="35"/>
-    </row>
-    <row r="22" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="H21" s="66"/>
+    </row>
+    <row r="22" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>11</v>
       </c>
@@ -1355,6 +1481,7 @@
       </c>
       <c r="F22" s="31"/>
       <c r="G22" s="36"/>
+      <c r="H22" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>